<commit_message>
r script demo data
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/R script/demographic data/data/data_empschul_labor_lehrperson_2021-11-24.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/R script/demographic data/data/data_empschul_labor_lehrperson_2021-11-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\R script\demographic data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_4BA6F5451BDC24510042E4A75C65406E9A9BF291" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0DDCBA05-00D1-4C71-B0C1-94BD7824A620}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_4BA6F5451BDC24510042E4A75C65406E9A9BF291" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{6939118B-BA34-4EEC-9860-2F6E5441A733}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,12 +668,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS1" sqref="AS1"/>
+      <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="4" width="20" customWidth="1"/>
@@ -695,7 +695,7 @@
     <col min="63" max="1024" width="11.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -883,7 +883,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>98</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>24</v>
       </c>
       <c r="AK3" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AL3" s="2" t="s">
         <v>64</v>
@@ -1243,7 +1243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>101</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>104</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>109</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>110</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>111</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>112</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>113</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>114</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>116</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>118</v>
       </c>

</xml_diff>